<commit_message>
v1.1 add requirements.txt, add verbose option, minor revisions in readme.md and input.xlsx
</commit_message>
<xml_diff>
--- a/input_setting/input.xlsx
+++ b/input_setting/input.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\00.Study_Projects\drug_patent_tracker\input_setting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76479688-7997-4DBC-8E34-C9D9F5D88399}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67B7FDFB-934E-4AD8-8FAD-98F4190DD472}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7965" yWindow="2640" windowWidth="17460" windowHeight="12150" xr2:uid="{87609493-9442-4A22-9039-ADBA54803282}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15620" activeTab="2" xr2:uid="{87609493-9442-4A22-9039-ADBA54803282}"/>
   </bookViews>
   <sheets>
     <sheet name="targets" sheetId="1" r:id="rId1"/>
     <sheet name="dates" sheetId="2" r:id="rId2"/>
-    <sheet name="output_mode" sheetId="3" r:id="rId3"/>
+    <sheet name="output_type" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
   <si>
     <t>출원번호</t>
   </si>
@@ -162,6 +162,10 @@
   </si>
   <si>
     <t>김수용</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>api key</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -228,7 +232,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -238,6 +242,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -256,7 +272,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -284,38 +300,44 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -633,53 +655,53 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E009A200-6AB0-454D-A8F9-4AEAABC1266A}">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="15.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.58203125" style="7" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="48.5" style="7" customWidth="1"/>
-    <col min="3" max="3" width="12.375" style="7" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" style="7" customWidth="1"/>
     <col min="4" max="4" width="13.75" style="7" customWidth="1"/>
     <col min="5" max="5" width="9.75" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.125" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.08203125" style="7" bestFit="1" customWidth="1"/>
     <col min="7" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" s="5"/>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="9" t="s">
         <v>17</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="18">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A3" s="15">
         <v>1020197005490</v>
       </c>
       <c r="B3" t="s">
@@ -698,8 +720,8 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="18">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A4" s="15">
         <v>1020207019364</v>
       </c>
       <c r="B4" t="s">
@@ -718,8 +740,8 @@
         <v>5678</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="18">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A5" s="15">
         <v>1020077026801</v>
       </c>
       <c r="B5" t="s">
@@ -738,8 +760,8 @@
         <v>1011</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="18">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A6" s="15">
         <v>1020187023203</v>
       </c>
       <c r="B6" t="s">
@@ -758,8 +780,8 @@
         <v>1112</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="18">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A7" s="15">
         <v>1020180173064</v>
       </c>
       <c r="B7" t="s">
@@ -778,26 +800,26 @@
         <v>1213</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="10"/>
-      <c r="B8" s="13"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="11"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A8" s="9"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="10"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9"/>
       <c r="B9" s="8"/>
-      <c r="F9" s="12"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F9" s="11"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="F10"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="F11"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="F12"/>
     </row>
   </sheetData>
@@ -815,26 +837,26 @@
   <dimension ref="B2:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="9" style="1"/>
-    <col min="2" max="2" width="13.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.08203125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="17">
+      <c r="C2" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B3" s="3" t="s">
         <v>4</v>
       </c>
@@ -842,7 +864,7 @@
         <v>41699</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B4" s="4" t="s">
         <v>5</v>
       </c>
@@ -859,42 +881,52 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0C47007-5539-4B93-829F-B9FD91FD0F0B}">
-  <dimension ref="B1:C4"/>
+  <dimension ref="B3:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="9" style="1"/>
     <col min="2" max="2" width="12.75" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="9" style="1"/>
+    <col min="3" max="4" width="9" style="1"/>
+    <col min="5" max="5" width="70.58203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B1" s="16" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B2" s="14" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B3" s="15"/>
-    </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B3" s="13"/>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B4" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="19" t="s">
         <v>10</v>
+      </c>
+      <c r="D4" s="17"/>
+      <c r="E4" s="16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="E5" s="18" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B7" s="21"/>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B8" s="1" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>